<commit_message>
updated DB to reflect current taps. Added location to all items. Entered HH y/n for all items.
</commit_message>
<xml_diff>
--- a/taplistDB.xlsx
+++ b/taplistDB.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="517"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="517"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$L$54</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="227">
   <si>
     <t>TAP</t>
   </si>
@@ -92,9 +92,6 @@
     <t>\</t>
   </si>
   <si>
-    <t>Omission</t>
-  </si>
-  <si>
     <t>Gluten Free - IPA</t>
   </si>
   <si>
@@ -110,15 +107,6 @@
     <t>Cabernet</t>
   </si>
   <si>
-    <t>Milbrandt</t>
-  </si>
-  <si>
-    <t>2011, black cherry, blackberry, cassis, mocha</t>
-  </si>
-  <si>
-    <t>Spire</t>
-  </si>
-  <si>
     <t>Spiced Apple</t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>Sauvignon Blanc</t>
   </si>
   <si>
-    <t>Proletariat</t>
-  </si>
-  <si>
     <t>Sauv Blanc 2013</t>
   </si>
   <si>
@@ -221,18 +206,9 @@
     <t>Chardonnay</t>
   </si>
   <si>
-    <t>Glacier Rock</t>
-  </si>
-  <si>
-    <t>2012 fresh and vibrant, apple, pear, vanilla</t>
-  </si>
-  <si>
     <t>Carbonated Wine</t>
   </si>
   <si>
-    <t>Hi-Wheel</t>
-  </si>
-  <si>
     <t>Lavender Lemon</t>
   </si>
   <si>
@@ -497,13 +473,244 @@
     <t>gluten-free</t>
   </si>
   <si>
-    <t>Vin Mousseux</t>
+    <t>Hood River, OR</t>
+  </si>
+  <si>
+    <t>Leavenworth, WA</t>
+  </si>
+  <si>
+    <t>San Diego, CA</t>
+  </si>
+  <si>
+    <t>Boise, ID.</t>
+  </si>
+  <si>
+    <t>Seattle, WA</t>
+  </si>
+  <si>
+    <t>Baker City, OR</t>
+  </si>
+  <si>
+    <t>Petaluma, CA</t>
+  </si>
+  <si>
+    <t>Escondito, CA</t>
+  </si>
+  <si>
+    <t>Baltimore, MD</t>
+  </si>
+  <si>
+    <t>Pacific, WA</t>
+  </si>
+  <si>
+    <t>Corvallis, OR</t>
+  </si>
+  <si>
+    <t>Denver, CO</t>
+  </si>
+  <si>
+    <t>Hi-Wheel Wine &amp; Mead Company</t>
+  </si>
+  <si>
+    <t>Spire Mountain (Fish Brewing Company)</t>
+  </si>
+  <si>
+    <t>Olympia, WA</t>
+  </si>
+  <si>
+    <t>Proletariat Wine Company</t>
+  </si>
+  <si>
+    <t>Walla Walla, WA</t>
+  </si>
+  <si>
+    <t>Milbrandt Vineyards</t>
+  </si>
+  <si>
+    <t>Prosser, WA</t>
+  </si>
+  <si>
+    <t>Jalliance</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Widmer Brothers Brewing</t>
+  </si>
+  <si>
+    <t>6 oz glass</t>
+  </si>
+  <si>
+    <t>Baltic-style Porter</t>
+  </si>
+  <si>
+    <t>21st Amendment Brewery</t>
+  </si>
+  <si>
+    <t>He Said</t>
+  </si>
+  <si>
+    <t>12 oz snifter</t>
+  </si>
+  <si>
+    <t>He Said is a black Baltic-Style Porter lager brewed with pumpkin, Vietnamese cinnamon and ground caraway</t>
+  </si>
+  <si>
+    <t>California Lager</t>
+  </si>
+  <si>
+    <t>Made in San Francisco with two-row California barley, Cluster hops and Anchor's own lager yeast.</t>
+  </si>
+  <si>
+    <t>East Side Oatmeal Pilsner</t>
+  </si>
+  <si>
+    <t> Lots of German pils character but with supercharged hop flavors and aromas from Czech Saaz and Santiam hops.</t>
+  </si>
+  <si>
+    <t>Pilsner</t>
+  </si>
+  <si>
+    <t>Country Boy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry, Clean, Crisp, and very Citrusy. This beer is made for the hop lovers. Centennial, Amarillo, and Cluster hops provide a wonderful hop aroma and flavor in this beer. </t>
+  </si>
+  <si>
+    <t>Hopworks Urban Brewery</t>
+  </si>
+  <si>
+    <t>Everybody's Brewing</t>
+  </si>
+  <si>
+    <t>Single Hop IPX Fuggle</t>
+  </si>
+  <si>
+    <t> This series highlights signature flavors of specific dry-hopped varieties. This one brewed with Fuggle hops, it is spicy, woody &amp; earthy</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>Nitro Cyclops</t>
+  </si>
+  <si>
+    <t> A cornucopia of 5 hop varieties, which yield striking flavor and aroma, that results in one of the more balanced and aromatic IPA</t>
+  </si>
+  <si>
+    <t>Nitro IPA</t>
+  </si>
+  <si>
+    <t>Cascade Lakes</t>
+  </si>
+  <si>
+    <t>Wild Turkey Stout</t>
+  </si>
+  <si>
+    <t>Woody, vanilla notes, fresh baked bread, toffee, and espresso, rich chocolate and roasted barley flavors.</t>
+  </si>
+  <si>
+    <t>Boiled and dry hopped using 4 NW hop varietals. Pineapple and citrus notes. Prepare yourself for a wild ride…Rev it up with the RPM IPA</t>
+  </si>
+  <si>
+    <t>Boonville, CA</t>
+  </si>
+  <si>
+    <t>Anderson Valley</t>
+  </si>
+  <si>
+    <t>Stout</t>
+  </si>
+  <si>
+    <t>Sourpuss</t>
+  </si>
+  <si>
+    <t>From Lake Oswego with notes of fruit and plenty of lactic sourness. A refreshing drink and very low alcohol make for an all day drinking beer.</t>
+  </si>
+  <si>
+    <t>Lake Oswego, OR</t>
+  </si>
+  <si>
+    <t>Stickmen</t>
+  </si>
+  <si>
+    <t>Yvan the Great</t>
+  </si>
+  <si>
+    <t>This beer has the bright, resinous hop profile of an American IPA blended with the dry and complex yeast character of a Belgian farmhouse ale.</t>
+  </si>
+  <si>
+    <t>Belgian-style Blonde</t>
+  </si>
+  <si>
+    <t>Sierra Nevada</t>
+  </si>
+  <si>
+    <t>Dry Hopped Cider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some say its like chewing on grass, others say its like drinking a meadow. Organic Cascade hops flavor this off cider. </t>
+  </si>
+  <si>
+    <t>Chimacum, WA</t>
+  </si>
+  <si>
+    <t>Finn River</t>
+  </si>
+  <si>
+    <t>Tent Show: Holy Water-Melon</t>
+  </si>
+  <si>
+    <t>Granny Smith apples, ginger, lime and lots and lots of watermelon!</t>
+  </si>
+  <si>
+    <t>Riesling</t>
+  </si>
+  <si>
+    <t>Glacier Rock Riesling</t>
+  </si>
+  <si>
+    <t>Well-balanced with exotic aromas and flavors of ripe nectarine, white peach, spicy jasmine and a hint of minerality that combine subtle sweetness with a crisp, refreshing finish</t>
+  </si>
+  <si>
+    <t>Glacier Rock Chardonnay</t>
+  </si>
+  <si>
+    <t>2012, Fresh and vibrant with aromas and flavors of apple, pear and hints of vanilla giving way to a crisp finish</t>
+  </si>
+  <si>
+    <t>Cabernet cuvee</t>
+  </si>
+  <si>
+    <t>2010, Delivers flavors of black cherry, plum, cassis, mocha and blueberry, with a lengthy, smooth finish</t>
+  </si>
+  <si>
+    <t>Terra Blanca</t>
+  </si>
+  <si>
+    <t>Benton City, WA</t>
+  </si>
+  <si>
+    <t>Terrace Triple Threat</t>
+  </si>
+  <si>
+    <t>Anchor Brewing</t>
+  </si>
+  <si>
+    <t>White Salmon, WA</t>
+  </si>
+  <si>
+    <t>Redmond, OR</t>
+  </si>
+  <si>
+    <t>Chico, CA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -512,20 +719,12 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -559,17 +758,42 @@
     <font>
       <sz val="12"/>
       <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF141823"/>
+      <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -577,36 +801,14 @@
       <sz val="12"/>
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Cambria"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Cambria"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="8"/>
+      <color theme="1" tint="0.14999847407452621"/>
       <name val="Cambria"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Cambria"/>
+      <family val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -635,302 +837,329 @@
   </borders>
   <cellStyleXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1435,7 +1664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1443,33 +1672,33 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="20"/>
-    <col min="3" max="3" width="10.6640625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="17" style="20" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="20" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="20" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" style="24" customWidth="1"/>
-    <col min="9" max="9" width="6.1640625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="20" customWidth="1"/>
-    <col min="11" max="11" width="8" style="25" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="26" customWidth="1"/>
-    <col min="13" max="13" width="86.6640625" style="28" customWidth="1"/>
-    <col min="14" max="16384" width="8.6640625" style="20"/>
+    <col min="1" max="1" width="6.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="4"/>
+    <col min="3" max="3" width="10.625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="32" customWidth="1"/>
+    <col min="9" max="9" width="6.125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8" style="38" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="39" customWidth="1"/>
+    <col min="13" max="13" width="86.625" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="8.625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="8" customFormat="1">
+    <row r="1" spans="1:18" s="17" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1478,91 +1707,93 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="10" customFormat="1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="M1" s="27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="10" customFormat="1">
-      <c r="A2" s="1">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="13">
+        <v>69</v>
+      </c>
+      <c r="H2" s="24">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="20">
         <v>4.75</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="3">
         <v>10</v>
       </c>
-      <c r="M2" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" s="8" customFormat="1">
+      <c r="M2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="17" customFormat="1">
       <c r="A3" s="1">
         <v>10</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>134</v>
+      <c r="B3" s="17" t="s">
+        <v>126</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="F3" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H3" s="13">
+        <v>78</v>
+      </c>
+      <c r="H3" s="24">
         <v>0.04</v>
       </c>
       <c r="I3" s="1">
@@ -1571,38 +1802,40 @@
       <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="19">
+      <c r="K3" s="25">
         <v>4.75</v>
       </c>
-      <c r="L3" s="32">
+      <c r="L3" s="26">
         <v>10</v>
       </c>
-      <c r="M3" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="O3" s="11"/>
+      <c r="M3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:18" s="10" customFormat="1">
       <c r="A4" s="1">
         <v>13</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>134</v>
+      <c r="B4" s="17" t="s">
+        <v>126</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="F4" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="13">
+        <v>46</v>
+      </c>
+      <c r="H4" s="24">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="I4" s="1">
@@ -1611,38 +1844,40 @@
       <c r="J4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="25">
         <v>5.5</v>
       </c>
-      <c r="L4" s="32">
+      <c r="L4" s="26">
         <v>16</v>
       </c>
-      <c r="M4" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="O4" s="12"/>
+      <c r="M4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="28"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1">
       <c r="A5" s="1">
         <v>18</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>134</v>
+      <c r="B5" s="17" t="s">
+        <v>126</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>118</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H5" s="13">
+        <v>119</v>
+      </c>
+      <c r="H5" s="24">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="I5" s="1">
@@ -1651,78 +1886,78 @@
       <c r="J5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="20">
         <v>4.75</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="3">
         <v>14</v>
       </c>
-      <c r="M5" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="O5" s="12"/>
+      <c r="M5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O5" s="28"/>
     </row>
     <row r="6" spans="1:18" s="10" customFormat="1">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="13">
+        <v>55</v>
+      </c>
+      <c r="H6" s="24">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="20">
         <v>4.75</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="29">
         <v>10</v>
       </c>
-      <c r="M6" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="O6" s="12"/>
+      <c r="M6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="10" customFormat="1">
-      <c r="A7" s="1">
-        <v>9</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" s="13">
+        <v>83</v>
+      </c>
+      <c r="H7" s="24">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="I7" s="1">
@@ -1731,79 +1966,79 @@
       <c r="J7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="20">
         <v>4.75</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="29">
         <v>10</v>
       </c>
-      <c r="M7" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="12"/>
+      <c r="M7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N7" s="17"/>
+      <c r="O7" s="28"/>
     </row>
     <row r="8" spans="1:18" s="10" customFormat="1">
       <c r="A8" s="1">
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H8" s="13">
+        <v>109</v>
+      </c>
+      <c r="H8" s="24">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="20">
         <v>4.5</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="3">
         <v>14</v>
       </c>
-      <c r="M8" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="O8" s="12"/>
-    </row>
-    <row r="9" spans="1:18" s="8" customFormat="1">
-      <c r="A9" s="1">
-        <v>4</v>
-      </c>
+      <c r="M8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O8" s="28"/>
+    </row>
+    <row r="9" spans="1:18" s="17" customFormat="1">
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="13">
+        <v>100</v>
+      </c>
+      <c r="H9" s="24">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="I9" s="1">
@@ -1812,40 +2047,38 @@
       <c r="J9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="20">
         <v>5.5</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="29">
         <v>16</v>
       </c>
-      <c r="M9" s="15" t="s">
-        <v>109</v>
+      <c r="M9" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:18" s="10" customFormat="1">
-      <c r="A10" s="1">
-        <v>5</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H10" s="13">
+        <v>98</v>
+      </c>
+      <c r="H10" s="24">
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="I10" s="1">
@@ -1854,78 +2087,82 @@
       <c r="J10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="20">
         <v>5</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="29">
         <v>16</v>
       </c>
-      <c r="M10" s="15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" s="8" customFormat="1">
+      <c r="M10" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="17" customFormat="1">
       <c r="A11" s="1">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="F11" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="13">
+        <v>58</v>
+      </c>
+      <c r="H11" s="24">
         <v>0.06</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="30">
         <v>43</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="20">
         <v>5.5</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="29">
         <v>16</v>
       </c>
-      <c r="M11" s="15" t="s">
-        <v>120</v>
+      <c r="M11" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
     </row>
-    <row r="12" spans="1:18" s="8" customFormat="1">
+    <row r="12" spans="1:18" s="17" customFormat="1">
       <c r="A12" s="1">
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>122</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H12" s="13">
+        <v>123</v>
+      </c>
+      <c r="H12" s="24">
         <v>7.8E-2</v>
       </c>
       <c r="I12" s="1">
@@ -1934,41 +2171,41 @@
       <c r="J12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="20">
         <v>4.5</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="3">
         <v>17</v>
       </c>
-      <c r="M12" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="N12" s="13"/>
+      <c r="M12" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N12" s="24"/>
       <c r="O12" s="10"/>
     </row>
-    <row r="13" spans="1:18" s="8" customFormat="1">
+    <row r="13" spans="1:18" s="17" customFormat="1">
       <c r="A13" s="1">
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H13" s="13">
+        <v>103</v>
+      </c>
+      <c r="H13" s="24">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I13" s="1">
@@ -1977,14 +2214,14 @@
       <c r="J13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="20">
         <v>4.75</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="3">
         <v>15</v>
       </c>
-      <c r="M13" s="15" t="s">
-        <v>145</v>
+      <c r="M13" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1994,22 +2231,24 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" s="13">
+        <v>88</v>
+      </c>
+      <c r="H14" s="24">
         <v>0.09</v>
       </c>
       <c r="I14" s="1">
@@ -2018,57 +2257,55 @@
       <c r="J14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="20">
         <v>4.75</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="3">
         <v>14</v>
       </c>
-      <c r="M14" s="15" t="s">
-        <v>121</v>
+      <c r="M14" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="7"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="3"/>
     </row>
     <row r="15" spans="1:18" s="10" customFormat="1">
-      <c r="A15" s="1">
-        <v>26</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" s="13">
+        <v>75</v>
+      </c>
+      <c r="H15" s="24">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="20">
         <v>4.75</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="15" t="s">
-        <v>147</v>
+      <c r="M15" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="10" customFormat="1">
@@ -2076,69 +2313,75 @@
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="G16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H16" s="13">
+        <v>91</v>
+      </c>
+      <c r="H16" s="24">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="20">
         <v>4.75</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="29">
         <v>16</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:15" s="10" customFormat="1">
-      <c r="A17" s="1">
-        <v>2</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="G17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="13">
+        <v>72</v>
+      </c>
+      <c r="H17" s="24">
         <v>0.09</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="25">
         <v>5</v>
       </c>
-      <c r="L17" s="32" t="s">
+      <c r="L17" s="26" t="s">
         <v>10</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:15" s="10" customFormat="1">
@@ -2146,36 +2389,40 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="G18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" s="2">
+        <v>49</v>
+      </c>
+      <c r="H18" s="7">
         <v>5.5E-2</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="6">
         <v>20</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="9">
         <v>5</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="3">
         <v>16</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="10" customFormat="1">
@@ -2183,34 +2430,38 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="G19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="13">
+        <v>66</v>
+      </c>
+      <c r="H19" s="24">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="20">
         <v>4.75</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="29">
         <v>12</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:15" s="10" customFormat="1">
@@ -2218,34 +2469,38 @@
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+        <v>94</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="G20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H20" s="13">
+        <v>95</v>
+      </c>
+      <c r="H20" s="24">
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="20">
         <v>5</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="3">
         <v>14</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:15" s="10" customFormat="1">
@@ -2253,24 +2508,24 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="13">
+        <v>35</v>
+      </c>
+      <c r="H21" s="24">
         <v>0.03</v>
       </c>
       <c r="I21" s="1">
@@ -2279,14 +2534,14 @@
       <c r="J21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="20">
         <v>4.75</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="3">
         <v>15</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="10" customFormat="1">
@@ -2294,24 +2549,24 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="13">
+        <v>84</v>
+      </c>
+      <c r="H22" s="24">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="I22" s="1">
@@ -2320,130 +2575,127 @@
       <c r="J22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="20">
         <v>4.75</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="3">
         <v>15</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="N22" s="18"/>
+        <v>85</v>
+      </c>
+      <c r="N22" s="31"/>
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" s="1" customFormat="1">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
       <c r="B23" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="13">
+        <v>51</v>
+      </c>
+      <c r="H23" s="24">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="20">
         <v>7.5</v>
       </c>
-      <c r="L23" s="7" t="s">
+      <c r="L23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N23" s="18"/>
-    </row>
-    <row r="24" spans="1:15" s="8" customFormat="1">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="N23" s="31"/>
+    </row>
+    <row r="24" spans="1:15" s="17" customFormat="1">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="G24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H24" s="13">
+        <v>61</v>
+      </c>
+      <c r="H24" s="24">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="20">
         <v>6</v>
       </c>
-      <c r="L24" s="7" t="s">
+      <c r="L24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" s="8" customFormat="1">
-      <c r="A25" s="1">
-        <v>14</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>41</v>
+    <row r="25" spans="1:15" s="17" customFormat="1">
+      <c r="A25" s="1"/>
+      <c r="B25" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H25" s="13">
+        <v>38</v>
+      </c>
+      <c r="H25" s="24">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="20">
         <v>6</v>
       </c>
-      <c r="L25" s="14">
+      <c r="L25" s="29">
         <v>24</v>
       </c>
-      <c r="M25" s="20" t="s">
-        <v>114</v>
+      <c r="M25" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="N25" s="10"/>
       <c r="O25" s="1"/>
@@ -2452,426 +2704,954 @@
       <c r="A26" s="1">
         <v>17</v>
       </c>
-      <c r="B26" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="20" t="s">
+      <c r="B26" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="32">
+        <v>5.5E-2</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="33">
+        <v>4</v>
+      </c>
+      <c r="L26" s="3">
+        <v>10</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" s="31"/>
+      <c r="O26" s="17"/>
+    </row>
+    <row r="27" spans="1:15" s="31" customFormat="1">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20" t="s">
+      <c r="E27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="24">
-        <v>5.5E-2</v>
-      </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="K26" s="21">
-        <v>4</v>
-      </c>
-      <c r="L26" s="7">
-        <v>10</v>
-      </c>
-      <c r="M26" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="N26" s="18"/>
-      <c r="O26" s="8"/>
-    </row>
-    <row r="27" spans="1:15" s="18" customFormat="1">
-      <c r="A27" s="20">
-        <v>25</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" s="13">
+      <c r="H27" s="24">
         <v>6.3E-2</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="20">
         <v>7</v>
       </c>
-      <c r="L27" s="14">
+      <c r="L27" s="29">
         <v>24</v>
       </c>
-      <c r="M27" s="20" t="s">
-        <v>36</v>
+      <c r="M27" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="N27" s="1"/>
-      <c r="O27" s="8"/>
-    </row>
-    <row r="28" spans="1:15" s="18" customFormat="1">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
+      <c r="O27" s="17"/>
+    </row>
+    <row r="28" spans="1:15" s="31" customFormat="1">
+      <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>43</v>
+        <v>145</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="13">
+        <v>164</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="24">
         <v>0.13500000000000001</v>
       </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="6">
+      <c r="J28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K28" s="9">
         <v>7.5</v>
       </c>
-      <c r="L28" s="7" t="s">
+      <c r="L28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N28" s="1"/>
-      <c r="O28" s="17"/>
-    </row>
-    <row r="29" spans="1:15" s="18" customFormat="1">
+      <c r="O28" s="34"/>
+    </row>
+    <row r="29" spans="1:15" s="31" customFormat="1">
       <c r="A29" s="1">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="6">
+        <v>166</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H29" s="7">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="I29" s="6"/>
+      <c r="J29" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K29" s="9">
         <v>7.5</v>
       </c>
-      <c r="L29" s="7" t="s">
+      <c r="L29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M29" s="15"/>
+      <c r="M29" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="N29" s="1"/>
-      <c r="O29" s="19"/>
+      <c r="O29" s="25"/>
     </row>
     <row r="30" spans="1:15" s="1" customFormat="1">
       <c r="A30" s="1">
         <v>32</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="3"/>
-      <c r="K30" s="6">
+      <c r="E30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K30" s="9">
         <v>8</v>
       </c>
-      <c r="L30" s="7" t="s">
+      <c r="L30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M30" s="15"/>
-    </row>
-    <row r="31" spans="1:15" s="8" customFormat="1">
+      <c r="M30" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="17" customFormat="1">
       <c r="A31" s="1">
         <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>27</v>
+        <v>145</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="6">
+        <v>166</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="H31" s="7">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="I31" s="6"/>
+      <c r="J31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K31" s="9">
         <v>8.5</v>
       </c>
-      <c r="L31" s="7" t="s">
+      <c r="L31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M31" s="15"/>
-    </row>
-    <row r="32" spans="1:15" s="8" customFormat="1">
+      <c r="M31" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="17" customFormat="1">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C32" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="G32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="13"/>
+      <c r="H32" s="24"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K32" s="9">
+      <c r="K32" s="20">
         <v>2.5</v>
       </c>
-      <c r="L32" s="7" t="s">
+      <c r="L32" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M32" s="28"/>
-    </row>
-    <row r="33" spans="1:16" s="8" customFormat="1">
+      <c r="M32" s="4"/>
+    </row>
+    <row r="33" spans="1:16" s="17" customFormat="1">
       <c r="A33" s="1">
         <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="G33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H33" s="13"/>
+        <v>81</v>
+      </c>
+      <c r="H33" s="24"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K33" s="19">
+      <c r="K33" s="25">
         <v>6</v>
       </c>
-      <c r="L33" s="7" t="s">
+      <c r="L33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M33" s="28"/>
-    </row>
-    <row r="34" spans="1:16" s="8" customFormat="1">
+      <c r="M33" s="4"/>
+    </row>
+    <row r="34" spans="1:16" s="17" customFormat="1">
       <c r="A34" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C34" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" s="29" customFormat="1">
-      <c r="A35" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>156</v>
+      <c r="H34" s="7"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K34" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="35" customFormat="1">
+      <c r="A35" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H35" s="13">
+      <c r="H35" s="24">
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="I35" s="1">
         <v>65</v>
       </c>
       <c r="J35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="25">
+        <v>4.25</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M35" s="4"/>
+    </row>
+    <row r="36" spans="1:16" s="11" customFormat="1">
+      <c r="A36" s="10">
+        <v>2</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="H36" s="14">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="K36" s="15">
+        <v>7.5</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="M36" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="1">
+        <v>6</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="H37" s="19">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K37" s="20">
+        <v>5</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M37" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="1">
+        <v>9</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="H38" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="I38" s="18">
+        <v>50</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" s="21">
+        <v>4.75</v>
+      </c>
+      <c r="L38" s="22">
+        <v>15</v>
+      </c>
+      <c r="M38" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="1">
+        <v>4</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H39" s="24">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I39" s="1">
+        <v>80</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K39" s="20">
+        <v>5</v>
+      </c>
+      <c r="L39" s="29">
+        <v>16</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" s="1" customFormat="1">
+      <c r="A40" s="1">
+        <v>14</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H40" s="24">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="I40" s="1">
+        <v>60</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" s="20">
+        <v>5</v>
+      </c>
+      <c r="L40" s="29">
+        <v>15</v>
+      </c>
+      <c r="M40" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" s="1" customFormat="1">
+      <c r="A41" s="1">
+        <v>21</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H41" s="24">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>75</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K41" s="20">
+        <v>5</v>
+      </c>
+      <c r="L41" s="29">
+        <v>14</v>
+      </c>
+      <c r="M41" s="40" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" s="1" customFormat="1">
+      <c r="A42" s="1">
+        <v>26</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="H42" s="19">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="I42" s="18">
+        <v>65</v>
+      </c>
+      <c r="J42" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K42" s="20">
+        <v>5.5</v>
+      </c>
+      <c r="L42" s="3">
+        <v>17</v>
+      </c>
+      <c r="M42" s="18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" s="1" customFormat="1">
+      <c r="A43" s="1">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H43" s="24">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="K43" s="20">
+        <v>6</v>
+      </c>
+      <c r="L43" s="29">
+        <v>16</v>
+      </c>
+      <c r="M43" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" s="1" customFormat="1">
+      <c r="A44" s="1">
+        <v>1</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H44" s="7">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="I44" s="6"/>
+      <c r="J44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K44" s="9">
+        <v>4.75</v>
+      </c>
+      <c r="L44" s="3">
+        <v>16</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" s="1" customFormat="1">
+      <c r="A45" s="1">
+        <v>3</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H45" s="7">
+        <v>6.3E-2</v>
+      </c>
+      <c r="I45" s="6"/>
+      <c r="J45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K45" s="9">
+        <v>6</v>
+      </c>
+      <c r="L45" s="3">
+        <v>16</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="1">
+        <v>23</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G46" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="H46" s="42">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" s="33">
+        <v>6.5</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M46" s="41" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" s="1" customFormat="1">
+      <c r="A47" s="1">
         <v>25</v>
       </c>
-      <c r="K35" s="19">
-        <v>4.25</v>
-      </c>
-      <c r="L35" s="7" t="s">
+      <c r="B47" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H47" s="24">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="20">
+        <v>7</v>
+      </c>
+      <c r="L47" s="29">
+        <v>18</v>
+      </c>
+      <c r="M47" s="41" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" s="1" customFormat="1">
+      <c r="A48" s="1">
+        <v>27</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H48" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K48" s="20">
+        <v>7.5</v>
+      </c>
+      <c r="L48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M35" s="20"/>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="G36" s="20"/>
-      <c r="L36" s="33"/>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="14"/>
-      <c r="P38" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="22">
-      <c r="C39" s="4"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="7"/>
-    </row>
-    <row r="40" spans="1:16" s="1" customFormat="1">
-      <c r="M40" s="15"/>
-    </row>
-    <row r="41" spans="1:16" s="1" customFormat="1">
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="3"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="15"/>
-    </row>
-    <row r="42" spans="1:16" s="1" customFormat="1">
-      <c r="M42" s="15"/>
-    </row>
-    <row r="43" spans="1:16" s="1" customFormat="1">
-      <c r="M43" s="15"/>
-    </row>
-    <row r="44" spans="1:16" s="1" customFormat="1">
-      <c r="M44" s="15"/>
-    </row>
-    <row r="45" spans="1:16" s="1" customFormat="1">
-      <c r="M45" s="15"/>
-    </row>
-    <row r="46" spans="1:16" ht="22">
-      <c r="C46" s="4"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="7"/>
-    </row>
-    <row r="47" spans="1:16" s="1" customFormat="1">
-      <c r="M47" s="15"/>
-    </row>
-    <row r="48" spans="1:16" s="1" customFormat="1">
-      <c r="M48" s="15"/>
-    </row>
-    <row r="49" spans="1:13" s="1" customFormat="1">
-      <c r="H49" s="13"/>
-      <c r="K49" s="19"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="15"/>
-    </row>
-    <row r="50" spans="1:13" s="1" customFormat="1">
-      <c r="M50" s="15"/>
-    </row>
-    <row r="51" spans="1:13" s="1" customFormat="1">
-      <c r="H51" s="13"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="15"/>
-    </row>
-    <row r="52" spans="1:13" ht="17">
-      <c r="A52" s="20"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="31"/>
-      <c r="I52" s="31"/>
-      <c r="J52" s="31"/>
-      <c r="K52" s="31"/>
-      <c r="L52" s="31"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53" s="20"/>
+      <c r="M48" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="1" customFormat="1">
+      <c r="A49" s="1">
+        <v>32</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H49" s="24"/>
+      <c r="J49" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K49" s="25">
+        <v>8</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="1" customFormat="1"/>
+    <row r="51" spans="1:12" s="1" customFormat="1">
+      <c r="H51" s="24"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="3"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="4"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="4"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -2883,19 +3663,19 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="57" spans="1:13">
-      <c r="C57" s="22"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="22"/>
-      <c r="I57" s="22"/>
-      <c r="J57" s="22"/>
-      <c r="K57" s="22"/>
-      <c r="L57" s="22"/>
-    </row>
-    <row r="58" spans="1:13">
+    <row r="57" spans="1:12">
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
+    </row>
+    <row r="58" spans="1:12">
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -2907,26 +3687,26 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:13">
-      <c r="A59" s="22"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="K59" s="20"/>
-      <c r="L59" s="20"/>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="G60" s="20"/>
-      <c r="H60" s="20"/>
-      <c r="K60" s="20"/>
-      <c r="L60" s="20"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="20"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="20"/>
-    </row>
-    <row r="63" spans="1:13">
+    <row r="59" spans="1:12">
+      <c r="A59" s="37"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" spans="1:12">
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -2938,19 +3718,19 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:13">
-      <c r="G64" s="20"/>
-      <c r="H64" s="20"/>
-      <c r="K64" s="20"/>
-      <c r="L64" s="20"/>
+    <row r="64" spans="1:12">
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="20"/>
+      <c r="A66" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="77" orientation="portrait"/>
+  <pageSetup paperSize="5" scale="77" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2961,16 +3741,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25"/>
   <sheetData/>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2981,16 +3761,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25"/>
   <sheetData/>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>